<commit_message>
Review for 2019.10.2 is done.
</commit_message>
<xml_diff>
--- a/作业打分.xlsx
+++ b/作业打分.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ganler-mac/Desktop/Dropbox/Ganler_Dropbox/COMPETITION/RM2020/招人和培训/SPTraining-VisionGroup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FF603C-3049-7946-A987-0F3E833FA14C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7BD937-BDE6-FF48-B701-89C7B66EA660}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{76E2E8F9-87E2-9C4F-9C6E-F35B2F867F25}"/>
   </bookViews>
@@ -124,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,7 +231,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -246,6 +252,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,7 +573,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -720,7 +729,7 @@
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="7">
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
@@ -754,7 +763,7 @@
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="7">
         <v>8</v>
       </c>
       <c r="C12" s="1"/>
@@ -788,7 +797,9 @@
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="7">
+        <v>9</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -852,7 +863,7 @@
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="7">
         <v>7.5</v>
       </c>
       <c r="C18" s="1"/>

</xml_diff>

<commit_message>
Check for week1 => ending
</commit_message>
<xml_diff>
--- a/作业打分.xlsx
+++ b/作业打分.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ganler-mac/Desktop/Dropbox/Ganler_Dropbox/COMPETITION/RM2020/招人和培训/SPTraining-VisionGroup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE23C2B-AC88-C744-AA85-6E8FC3BB0D31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35B3724-33F2-664A-9222-49CAE707CF3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{76E2E8F9-87E2-9C4F-9C6E-F35B2F867F25}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{76E2E8F9-87E2-9C4F-9C6E-F35B2F867F25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,8 +131,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,12 +164,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -253,7 +255,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -272,17 +274,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -602,7 +601,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -664,7 +663,9 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="7">
+        <v>7.5</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -698,7 +699,9 @@
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="7">
+        <v>7.5</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -714,7 +717,7 @@
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -730,7 +733,7 @@
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -746,7 +749,7 @@
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -780,7 +783,9 @@
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="7">
+        <v>7</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -814,7 +819,9 @@
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="7">
+        <v>8</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -866,7 +873,9 @@
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="7">
+        <v>8</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -918,7 +927,9 @@
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="7">
+        <v>8</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -934,7 +945,7 @@
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>7.5</v>
       </c>
       <c r="C20" s="1"/>

</xml_diff>